<commit_message>
readme update and html correction
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -507,13 +507,13 @@
         <v>668</v>
       </c>
       <c r="G2" t="n">
-        <v>1182</v>
+        <v>1169</v>
       </c>
       <c r="H2" t="n">
         <v>13</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -542,13 +542,13 @@
         <v>795</v>
       </c>
       <c r="G3" t="n">
-        <v>1358</v>
+        <v>1295</v>
       </c>
       <c r="H3" t="n">
         <v>13</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -648,122 +648,122 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Initial stock_x</t>
+          <t>Initial stock 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Demand_x</t>
+          <t>Demand 1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock_x</t>
+          <t>Final Stock 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Stock outs_x</t>
+          <t>Stock outs 1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock After Replenishment_x</t>
+          <t>Final Stock After Replenishment 1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Order size_x</t>
+          <t>Order size 1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Initial stock_y</t>
+          <t>Initial stock 2</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Demand_y</t>
+          <t>Demand 2</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock_y</t>
+          <t>Final Stock 2</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Stock outs_y</t>
+          <t>Stock outs 2</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock After Replenishment_y</t>
+          <t>Final Stock After Replenishment 2</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Order size_y</t>
+          <t>Order size 2</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Initial stock_x</t>
+          <t>Initial stock 3</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Demand_x</t>
+          <t>Demand 3</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock_x</t>
+          <t>Final Stock 3</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Stock outs_x</t>
+          <t>Stock outs 3</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock After Replenishment_x</t>
+          <t>Final Stock After Replenishment 3</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Order size_x</t>
+          <t>Order size 3</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Initial stock_y</t>
+          <t>Initial stock 4</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Demand_y</t>
+          <t>Demand 4</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock_y</t>
+          <t>Final Stock 4</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Stock outs_y</t>
+          <t>Stock outs 4</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Final Stock After Replenishment_y</t>
+          <t>Final Stock After Replenishment 4</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Order size_y</t>
+          <t>Order size 4</t>
         </is>
       </c>
     </row>
@@ -780,18 +780,18 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>445</t>
+          <t>375</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -806,18 +806,18 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>445</t>
+          <t>375</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -832,18 +832,18 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>445</t>
+          <t>375</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -858,18 +858,18 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>445</t>
+          <t>375</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -886,23 +886,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1175</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -912,23 +912,23 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>456</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>1175</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -938,23 +938,23 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>456</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -964,23 +964,23 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>625</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>456</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -997,23 +997,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1175</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>434</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1023,23 +1023,23 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1175</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>434</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -1049,17 +1049,17 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>434</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>-321</t>
+          <t>-265</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1079,17 +1079,17 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>169</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>434</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>-321</t>
+          <t>-265</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1116,23 +1116,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>485</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1142,23 +1142,23 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>485</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1168,23 +1168,23 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>485</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -1194,23 +1194,23 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>679</t>
+          <t>735</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>485</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1227,17 +1227,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>489</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>761</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1257,23 +1257,23 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>489</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>761</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>761</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1283,17 +1283,17 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>489</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1313,17 +1313,17 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>250</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>489</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1350,23 +1350,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>761</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>492</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1376,23 +1376,23 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>761</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>492</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>1267</t>
+          <t>1269</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1402,17 +1402,17 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>492</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>-733</t>
+          <t>-731</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1432,17 +1432,17 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>-310</t>
+          <t>-239</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>492</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>-733</t>
+          <t>-731</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -1469,17 +1469,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>540</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>729</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1499,43 +1499,43 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1267</t>
+          <t>1269</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>540</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>729</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>729</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>540</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1555,17 +1555,17 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>269</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>540</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1592,23 +1592,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>729</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>220</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>220</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1618,43 +1618,43 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>883</t>
+          <t>729</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>509</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>220</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>1220</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>509</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1674,17 +1674,17 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>-117</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>509</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1711,23 +1711,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>220</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>420</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>-200</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1026</t>
+          <t>800</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1737,23 +1741,23 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>1220</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>420</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>800</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1026</t>
+          <t>800</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1763,17 +1767,17 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>420</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>-974</t>
+          <t>-1200</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1783,7 +1787,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>-200</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1793,17 +1797,17 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>-582</t>
+          <t>-780</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>420</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>-974</t>
+          <t>-1200</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1813,7 +1817,7 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>-200</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1830,23 +1834,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1026</t>
+          <t>800</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>358</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1856,23 +1860,23 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1026</t>
+          <t>800</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>358</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1882,17 +1886,17 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>-200</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>358</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1902,7 +1906,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1912,17 +1916,17 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>-200</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>358</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -1932,7 +1936,7 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -1949,23 +1953,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>453</t>
+          <t>486</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>67</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>-44</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1067</t>
+          <t>956</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1975,23 +1983,27 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>442</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>453</t>
+          <t>486</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>67</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
+          <t>-44</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1067</t>
+          <t>956</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -2001,17 +2013,17 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>453</t>
+          <t>486</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -2021,7 +2033,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -2031,17 +2043,17 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-558</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>453</t>
+          <t>486</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -2051,7 +2063,7 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -2068,23 +2080,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1067</t>
+          <t>956</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>523</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -2094,23 +2106,23 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1067</t>
+          <t>956</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>523</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -2120,17 +2132,17 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>523</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>-1450</t>
+          <t>-1567</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -2140,7 +2152,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-567</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -2150,17 +2162,17 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>-933</t>
+          <t>-1044</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>523</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>-1450</t>
+          <t>-1567</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -2170,7 +2182,7 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-567</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -2187,23 +2199,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>491</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>-58</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1045</t>
+          <t>942</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -2213,23 +2229,27 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>433</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>491</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
+          <t>-58</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1045</t>
+          <t>942</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2239,17 +2259,17 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-567</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>491</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -2259,7 +2279,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -2269,17 +2289,17 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-567</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>491</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2289,7 +2309,7 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -2306,23 +2326,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1045</t>
+          <t>942</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>471</t>
+          <t>419</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -2332,23 +2352,23 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1045</t>
+          <t>942</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>471</t>
+          <t>419</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -2358,17 +2378,17 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>471</t>
+          <t>419</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -2378,7 +2398,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -2388,17 +2408,17 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>-955</t>
+          <t>-1058</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>471</t>
+          <t>419</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -2408,7 +2428,7 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2425,23 +2445,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>406</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>117</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>1117</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -2451,23 +2471,23 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>523</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>406</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>117</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>1117</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -2477,17 +2497,17 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>406</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>-1867</t>
+          <t>-1883</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -2497,7 +2517,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>-867</t>
+          <t>-883</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -2507,17 +2527,17 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>-1426</t>
+          <t>-1477</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>406</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>-1867</t>
+          <t>-1883</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -2527,7 +2547,7 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>-867</t>
+          <t>-883</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -2544,23 +2564,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>1117</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>433</t>
+          <t>409</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2570,23 +2590,23 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>1117</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>433</t>
+          <t>409</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2596,17 +2616,17 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>-867</t>
+          <t>-883</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>433</t>
+          <t>409</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -2616,7 +2636,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2626,17 +2646,17 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>-867</t>
+          <t>-883</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>433</t>
+          <t>409</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -2646,7 +2666,7 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2663,23 +2683,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>413</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>295</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>295</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2689,23 +2709,23 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>708</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>413</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>295</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>1295</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -2715,17 +2735,17 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>413</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -2735,7 +2755,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2745,17 +2765,17 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>-1300</t>
+          <t>-1292</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>413</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -2765,7 +2785,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2782,17 +2802,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>412</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>-245</t>
+          <t>-117</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2802,7 +2822,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>883</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2812,43 +2832,43 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>1295</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>412</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>883</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>883</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>412</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>-2245</t>
+          <t>-2117</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -2858,7 +2878,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>-1245</t>
+          <t>-1117</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2868,17 +2888,17 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1705</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>412</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>-2245</t>
+          <t>-2117</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -2888,7 +2908,7 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>-1245</t>
+          <t>-1117</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2905,23 +2925,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>883</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>357</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2931,43 +2951,43 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>883</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>357</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>-1245</t>
+          <t>-1117</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>357</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -2977,7 +2997,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2987,17 +3007,17 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>-1245</t>
+          <t>-1117</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>357</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -3007,7 +3027,7 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -3024,27 +3044,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>478</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>-61</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>1048</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -3054,23 +3070,23 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>526</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>478</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>48</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>1048</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -3080,17 +3096,17 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>478</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -3100,7 +3116,7 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -3110,17 +3126,17 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>-1700</t>
+          <t>-1474</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>478</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -3130,7 +3146,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -3147,23 +3163,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>1048</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>479</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -3173,23 +3189,23 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>1048</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>479</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -3199,17 +3215,17 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>479</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>-2463</t>
+          <t>-2431</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -3219,7 +3235,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>-1463</t>
+          <t>-1431</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -3229,17 +3245,17 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>-2061</t>
+          <t>-1952</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>479</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>-2463</t>
+          <t>-2431</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -3249,7 +3265,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>-1463</t>
+          <t>-1431</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -3266,23 +3282,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>407</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>162</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1162</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3292,23 +3308,23 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>569</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>407</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>162</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1162</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -3318,17 +3334,17 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>-1463</t>
+          <t>-1431</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>407</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -3338,7 +3354,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -3348,17 +3364,17 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>-1463</t>
+          <t>-1431</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>407</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
@@ -3368,7 +3384,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -3385,49 +3401,49 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1162</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>492</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1162</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>492</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -3437,17 +3453,17 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>492</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
@@ -3457,7 +3473,7 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
@@ -3467,17 +3483,17 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>-1920</t>
+          <t>-1838</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>492</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
@@ -3487,7 +3503,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3504,49 +3520,49 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>406</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>264</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>264</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>538</t>
+          <t>670</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>406</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>264</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>1264</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -3556,17 +3572,17 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>406</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>-2818</t>
+          <t>-2736</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -3576,7 +3592,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1736</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -3586,17 +3602,17 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>-2462</t>
+          <t>-2330</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>406</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>-2818</t>
+          <t>-2736</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -3606,7 +3622,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1736</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3623,23 +3639,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>264</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>464</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>739</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>-200</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>800</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -3649,43 +3669,43 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>1264</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>464</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>800</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>800</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1736</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>464</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
@@ -3695,7 +3715,7 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -3705,17 +3725,17 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>-1818</t>
+          <t>-1736</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>464</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
@@ -3725,7 +3745,7 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3742,23 +3762,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>800</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>375</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3768,43 +3788,43 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>800</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>375</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>375</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
@@ -3814,7 +3834,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -3824,17 +3844,17 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>-2261</t>
+          <t>-2200</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>375</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
@@ -3844,7 +3864,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3861,17 +3881,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>442</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>-79</t>
+          <t>-17</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3881,7 +3901,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>983</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -3891,23 +3911,27 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>425</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>442</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>921</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
+          <t>-17</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>983</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -3917,17 +3941,17 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>442</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>-3079</t>
+          <t>-3017</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
@@ -3937,7 +3961,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>-2079</t>
+          <t>-2017</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3947,17 +3971,17 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>-2642</t>
+          <t>-2575</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>442</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>-3079</t>
+          <t>-3017</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -3967,7 +3991,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>-2079</t>
+          <t>-2017</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3984,23 +4008,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>983</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>523</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -4010,23 +4034,23 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>983</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>523</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -4036,17 +4060,17 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>-2079</t>
+          <t>-2017</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>523</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -4056,7 +4080,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -4066,17 +4090,17 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>-2079</t>
+          <t>-2017</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>523</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
@@ -4086,7 +4110,7 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -4103,17 +4127,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>541</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>-77</t>
+          <t>-81</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -4123,7 +4147,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>923</t>
+          <t>919</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -4133,17 +4157,17 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>384</t>
+          <t>460</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>541</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>-77</t>
+          <t>-81</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -4153,7 +4177,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>923</t>
+          <t>919</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -4163,17 +4187,17 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>541</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -4183,7 +4207,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -4193,17 +4217,17 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>-2616</t>
+          <t>-2540</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>541</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
@@ -4213,7 +4237,7 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -4230,12 +4254,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>923</t>
+          <t>919</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>389</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -4256,12 +4280,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>923</t>
+          <t>919</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>389</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -4282,12 +4306,12 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>389</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -4312,12 +4336,12 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>-3077</t>
+          <t>-3081</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>389</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">

</xml_diff>